<commit_message>
add biogrid GO analysis results
biogrid background vs whole genome background
</commit_message>
<xml_diff>
--- a/docs/Anti-coronavirus-chemical-drugs-with_ontoIDs.xlsx
+++ b/docs/Anti-coronavirus-chemical-drugs-with_ontoIDs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\l_yin\Dropbox\Coronavirus drug paper prep\Submission to Scientific Data\manuscript for inquiry for Scientific Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e342ab95cc976646/文档/GitHub/anti-coronavirus-drugs/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78093CA-353F-4067-8B60-0BCF47FDD5EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{A78093CA-353F-4067-8B60-0BCF47FDD5EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A6EF4D44-CE12-4C90-A60F-C485B6D60001}"/>
   <bookViews>
-    <workbookView xWindow="6558" yWindow="2064" windowWidth="15096" windowHeight="6000" xr2:uid="{12B75FA6-2611-4C8D-BF03-8A2E9E357643}"/>
+    <workbookView xWindow="3162" yWindow="2298" windowWidth="13074" windowHeight="8406" xr2:uid="{12B75FA6-2611-4C8D-BF03-8A2E9E357643}"/>
   </bookViews>
   <sheets>
     <sheet name="Master data sheet" sheetId="1" r:id="rId1"/>
@@ -2011,8 +2011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B393D82-FB4B-43F8-874B-8DFEE9B0B148}">
   <dimension ref="A1:K181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="A92" sqref="A92"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>